<commit_message>
tested with 10 fold validation
</commit_message>
<xml_diff>
--- a/sentise_res.xlsx
+++ b/sentise_res.xlsx
@@ -685,9 +685,9 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="2.15234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="2.15234375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="2.15234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="3.375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="3.375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="3.375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -715,7 +715,7 @@
         <v>0.0</v>
       </c>
       <c r="D2" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="3">
@@ -723,7 +723,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -737,7 +737,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -751,13 +751,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="C5" t="n">
         <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="6">
@@ -765,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C6" t="n">
         <v>0.0</v>
@@ -782,10 +782,10 @@
         <v>0.0</v>
       </c>
       <c r="C7" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
@@ -793,7 +793,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -807,13 +807,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C9" t="n">
         <v>0.0</v>
       </c>
       <c r="D9" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="10">
@@ -821,7 +821,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C10" t="n">
         <v>0.0</v>
@@ -835,7 +835,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C11" t="n">
         <v>0.0</v>
@@ -849,7 +849,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C12" t="n">
         <v>0.0</v>
@@ -863,7 +863,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C13" t="n">
         <v>0.0</v>
@@ -877,7 +877,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -891,7 +891,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C15" t="n">
         <v>0.0</v>
@@ -905,7 +905,7 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C16" t="n">
         <v>0.0</v>
@@ -919,13 +919,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
@@ -933,7 +933,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C18" t="n">
         <v>0.0</v>
@@ -947,7 +947,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C19" t="n">
         <v>0.0</v>
@@ -961,7 +961,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
@@ -975,7 +975,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C21" t="n">
         <v>0.0</v>
@@ -989,7 +989,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C22" t="n">
         <v>0.0</v>
@@ -1003,7 +1003,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C23" t="n">
         <v>0.0</v>
@@ -1017,7 +1017,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C24" t="n">
         <v>0.0</v>
@@ -1031,7 +1031,7 @@
         <v>27</v>
       </c>
       <c r="B25" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C25" t="n">
         <v>0.0</v>
@@ -1045,7 +1045,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -1059,13 +1059,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="C27" t="n">
         <v>0.0</v>
       </c>
       <c r="D27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28">
@@ -1073,7 +1073,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C28" t="n">
         <v>0.0</v>
@@ -1087,7 +1087,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C29" t="n">
         <v>0.0</v>
@@ -1101,7 +1101,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C30" t="n">
         <v>0.0</v>
@@ -1115,7 +1115,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C31" t="n">
         <v>0.0</v>
@@ -1129,7 +1129,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C32" t="n">
         <v>0.0</v>
@@ -1143,7 +1143,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C33" t="n">
         <v>0.0</v>
@@ -1157,7 +1157,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C34" t="n">
         <v>0.0</v>
@@ -1171,7 +1171,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C35" t="n">
         <v>0.0</v>
@@ -1185,7 +1185,7 @@
         <v>38</v>
       </c>
       <c r="B36" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C36" t="n">
         <v>0.0</v>
@@ -1199,7 +1199,7 @@
         <v>39</v>
       </c>
       <c r="B37" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C37" t="n">
         <v>0.0</v>
@@ -1213,7 +1213,7 @@
         <v>40</v>
       </c>
       <c r="B38" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C38" t="n">
         <v>0.0</v>
@@ -1227,7 +1227,7 @@
         <v>41</v>
       </c>
       <c r="B39" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C39" t="n">
         <v>0.0</v>
@@ -1247,7 +1247,7 @@
         <v>0.0</v>
       </c>
       <c r="D40" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="41">
@@ -1255,13 +1255,13 @@
         <v>43</v>
       </c>
       <c r="B41" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="C41" t="n">
         <v>0.0</v>
       </c>
       <c r="D41" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="42">
@@ -1269,7 +1269,7 @@
         <v>44</v>
       </c>
       <c r="B42" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C42" t="n">
         <v>0.0</v>
@@ -1283,7 +1283,7 @@
         <v>45</v>
       </c>
       <c r="B43" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C43" t="n">
         <v>0.0</v>
@@ -1297,7 +1297,7 @@
         <v>46</v>
       </c>
       <c r="B44" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C44" t="n">
         <v>0.0</v>
@@ -1311,7 +1311,7 @@
         <v>47</v>
       </c>
       <c r="B45" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C45" t="n">
         <v>0.0</v>
@@ -1325,7 +1325,7 @@
         <v>48</v>
       </c>
       <c r="B46" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C46" t="n">
         <v>0.0</v>
@@ -1345,7 +1345,7 @@
         <v>0.0</v>
       </c>
       <c r="D47" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="48">
@@ -1353,7 +1353,7 @@
         <v>50</v>
       </c>
       <c r="B48" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C48" t="n">
         <v>0.0</v>
@@ -1367,7 +1367,7 @@
         <v>51</v>
       </c>
       <c r="B49" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C49" t="n">
         <v>0.0</v>
@@ -1381,7 +1381,7 @@
         <v>52</v>
       </c>
       <c r="B50" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C50" t="n">
         <v>0.0</v>
@@ -1395,7 +1395,7 @@
         <v>53</v>
       </c>
       <c r="B51" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C51" t="n">
         <v>0.0</v>
@@ -1409,13 +1409,13 @@
         <v>54</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C52" t="n">
         <v>0.0</v>
       </c>
       <c r="D52" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="53">
@@ -1426,7 +1426,7 @@
         <v>0.0</v>
       </c>
       <c r="C53" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="D53" t="n">
         <v>0.0</v>
@@ -1437,7 +1437,7 @@
         <v>56</v>
       </c>
       <c r="B54" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C54" t="n">
         <v>0.0</v>
@@ -1451,7 +1451,7 @@
         <v>57</v>
       </c>
       <c r="B55" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C55" t="n">
         <v>0.0</v>
@@ -1465,7 +1465,7 @@
         <v>58</v>
       </c>
       <c r="B56" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C56" t="n">
         <v>0.0</v>
@@ -1482,7 +1482,7 @@
         <v>0.0</v>
       </c>
       <c r="C57" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="D57" t="n">
         <v>0.0</v>
@@ -1493,7 +1493,7 @@
         <v>60</v>
       </c>
       <c r="B58" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C58" t="n">
         <v>0.0</v>
@@ -1507,7 +1507,7 @@
         <v>61</v>
       </c>
       <c r="B59" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C59" t="n">
         <v>0.0</v>
@@ -1521,7 +1521,7 @@
         <v>62</v>
       </c>
       <c r="B60" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C60" t="n">
         <v>0.0</v>
@@ -1535,13 +1535,13 @@
         <v>63</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="C61" t="n">
         <v>0.0</v>
       </c>
       <c r="D61" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="62">
@@ -1549,7 +1549,7 @@
         <v>64</v>
       </c>
       <c r="B62" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C62" t="n">
         <v>0.0</v>
@@ -1563,7 +1563,7 @@
         <v>65</v>
       </c>
       <c r="B63" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C63" t="n">
         <v>0.0</v>
@@ -1577,7 +1577,7 @@
         <v>66</v>
       </c>
       <c r="B64" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C64" t="n">
         <v>0.0</v>
@@ -1591,13 +1591,13 @@
         <v>67</v>
       </c>
       <c r="B65" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C65" t="n">
         <v>0.0</v>
       </c>
       <c r="D65" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="66">
@@ -1605,7 +1605,7 @@
         <v>68</v>
       </c>
       <c r="B66" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C66" t="n">
         <v>0.0</v>
@@ -1619,7 +1619,7 @@
         <v>69</v>
       </c>
       <c r="B67" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C67" t="n">
         <v>0.0</v>
@@ -1633,7 +1633,7 @@
         <v>70</v>
       </c>
       <c r="B68" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C68" t="n">
         <v>0.0</v>
@@ -1647,7 +1647,7 @@
         <v>71</v>
       </c>
       <c r="B69" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C69" t="n">
         <v>0.0</v>
@@ -1661,7 +1661,7 @@
         <v>72</v>
       </c>
       <c r="B70" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C70" t="n">
         <v>0.0</v>
@@ -1675,7 +1675,7 @@
         <v>73</v>
       </c>
       <c r="B71" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C71" t="n">
         <v>0.0</v>
@@ -1689,7 +1689,7 @@
         <v>74</v>
       </c>
       <c r="B72" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C72" t="n">
         <v>0.0</v>
@@ -1703,7 +1703,7 @@
         <v>75</v>
       </c>
       <c r="B73" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C73" t="n">
         <v>0.0</v>
@@ -1717,7 +1717,7 @@
         <v>76</v>
       </c>
       <c r="B74" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="C74" t="n">
         <v>0.0</v>
@@ -1731,7 +1731,7 @@
         <v>77</v>
       </c>
       <c r="B75" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C75" t="n">
         <v>0.0</v>
@@ -1745,7 +1745,7 @@
         <v>78</v>
       </c>
       <c r="B76" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C76" t="n">
         <v>0.0</v>
@@ -1759,13 +1759,13 @@
         <v>79</v>
       </c>
       <c r="B77" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C77" t="n">
         <v>0.0</v>
       </c>
       <c r="D77" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="78">
@@ -1773,10 +1773,10 @@
         <v>80</v>
       </c>
       <c r="B78" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C78" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="D78" t="n">
         <v>0.0</v>
@@ -1787,7 +1787,7 @@
         <v>81</v>
       </c>
       <c r="B79" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C79" t="n">
         <v>0.0</v>
@@ -1801,13 +1801,13 @@
         <v>82</v>
       </c>
       <c r="B80" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C80" t="n">
         <v>0.0</v>
       </c>
       <c r="D80" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="81">
@@ -1815,7 +1815,7 @@
         <v>83</v>
       </c>
       <c r="B81" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C81" t="n">
         <v>0.0</v>
@@ -1829,13 +1829,13 @@
         <v>84</v>
       </c>
       <c r="B82" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C82" t="n">
         <v>0.0</v>
       </c>
       <c r="D82" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="83">
@@ -1843,7 +1843,7 @@
         <v>85</v>
       </c>
       <c r="B83" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C83" t="n">
         <v>0.0</v>
@@ -1857,7 +1857,7 @@
         <v>86</v>
       </c>
       <c r="B84" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C84" t="n">
         <v>0.0</v>
@@ -1871,7 +1871,7 @@
         <v>87</v>
       </c>
       <c r="B85" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C85" t="n">
         <v>0.0</v>
@@ -1885,7 +1885,7 @@
         <v>88</v>
       </c>
       <c r="B86" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C86" t="n">
         <v>0.0</v>
@@ -1899,7 +1899,7 @@
         <v>89</v>
       </c>
       <c r="B87" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C87" t="n">
         <v>0.0</v>
@@ -1913,13 +1913,13 @@
         <v>90</v>
       </c>
       <c r="B88" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="C88" t="n">
         <v>0.0</v>
       </c>
       <c r="D88" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="89">
@@ -1927,7 +1927,7 @@
         <v>91</v>
       </c>
       <c r="B89" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C89" t="n">
         <v>0.0</v>
@@ -1941,7 +1941,7 @@
         <v>92</v>
       </c>
       <c r="B90" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C90" t="n">
         <v>0.0</v>
@@ -1955,7 +1955,7 @@
         <v>93</v>
       </c>
       <c r="B91" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C91" t="n">
         <v>0.0</v>
@@ -1969,10 +1969,10 @@
         <v>94</v>
       </c>
       <c r="B92" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D92" t="n">
         <v>0.0</v>
@@ -1983,7 +1983,7 @@
         <v>95</v>
       </c>
       <c r="B93" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C93" t="n">
         <v>0.0</v>
@@ -1997,7 +1997,7 @@
         <v>96</v>
       </c>
       <c r="B94" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C94" t="n">
         <v>0.0</v>
@@ -2011,7 +2011,7 @@
         <v>97</v>
       </c>
       <c r="B95" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C95" t="n">
         <v>0.0</v>
@@ -2025,7 +2025,7 @@
         <v>98</v>
       </c>
       <c r="B96" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C96" t="n">
         <v>0.0</v>
@@ -2039,7 +2039,7 @@
         <v>99</v>
       </c>
       <c r="B97" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C97" t="n">
         <v>0.0</v>
@@ -2053,7 +2053,7 @@
         <v>100</v>
       </c>
       <c r="B98" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C98" t="n">
         <v>0.0</v>
@@ -2067,7 +2067,7 @@
         <v>101</v>
       </c>
       <c r="B99" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C99" t="n">
         <v>0.0</v>
@@ -2081,13 +2081,13 @@
         <v>102</v>
       </c>
       <c r="B100" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C100" t="n">
         <v>0.0</v>
       </c>
       <c r="D100" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="101">
@@ -2095,13 +2095,13 @@
         <v>103</v>
       </c>
       <c r="B101" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C101" t="n">
         <v>0.0</v>
       </c>
       <c r="D101" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="102">
@@ -2109,13 +2109,13 @@
         <v>104</v>
       </c>
       <c r="B102" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="C102" t="n">
         <v>0.0</v>
       </c>
       <c r="D102" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="103">
@@ -2123,7 +2123,7 @@
         <v>105</v>
       </c>
       <c r="B103" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C103" t="n">
         <v>0.0</v>
@@ -2137,7 +2137,7 @@
         <v>106</v>
       </c>
       <c r="B104" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C104" t="n">
         <v>0.0</v>
@@ -2151,7 +2151,7 @@
         <v>107</v>
       </c>
       <c r="B105" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C105" t="n">
         <v>0.0</v>
@@ -2165,7 +2165,7 @@
         <v>108</v>
       </c>
       <c r="B106" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C106" t="n">
         <v>0.0</v>
@@ -2182,7 +2182,7 @@
         <v>0.0</v>
       </c>
       <c r="C107" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="D107" t="n">
         <v>0.0</v>
@@ -2193,13 +2193,13 @@
         <v>110</v>
       </c>
       <c r="B108" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C108" t="n">
         <v>0.0</v>
       </c>
       <c r="D108" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="109">
@@ -2207,13 +2207,13 @@
         <v>111</v>
       </c>
       <c r="B109" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="C109" t="n">
         <v>0.0</v>
       </c>
       <c r="D109" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="110">
@@ -2221,7 +2221,7 @@
         <v>112</v>
       </c>
       <c r="B110" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C110" t="n">
         <v>0.0</v>
@@ -2235,7 +2235,7 @@
         <v>113</v>
       </c>
       <c r="B111" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C111" t="n">
         <v>0.0</v>
@@ -2249,7 +2249,7 @@
         <v>114</v>
       </c>
       <c r="B112" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C112" t="n">
         <v>0.0</v>
@@ -2263,7 +2263,7 @@
         <v>115</v>
       </c>
       <c r="B113" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C113" t="n">
         <v>0.0</v>
@@ -2277,7 +2277,7 @@
         <v>116</v>
       </c>
       <c r="B114" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C114" t="n">
         <v>0.0</v>
@@ -2291,13 +2291,13 @@
         <v>117</v>
       </c>
       <c r="B115" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C115" t="n">
         <v>0.0</v>
       </c>
       <c r="D115" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="116">
@@ -2305,13 +2305,13 @@
         <v>118</v>
       </c>
       <c r="B116" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C116" t="n">
         <v>0.0</v>
       </c>
       <c r="D116" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="117">
@@ -2319,7 +2319,7 @@
         <v>119</v>
       </c>
       <c r="B117" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C117" t="n">
         <v>0.0</v>
@@ -2333,7 +2333,7 @@
         <v>120</v>
       </c>
       <c r="B118" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C118" t="n">
         <v>0.0</v>
@@ -2347,7 +2347,7 @@
         <v>121</v>
       </c>
       <c r="B119" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C119" t="n">
         <v>0.0</v>
@@ -2361,13 +2361,13 @@
         <v>122</v>
       </c>
       <c r="B120" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C120" t="n">
         <v>0.0</v>
       </c>
       <c r="D120" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="121">
@@ -2375,7 +2375,7 @@
         <v>123</v>
       </c>
       <c r="B121" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C121" t="n">
         <v>0.0</v>
@@ -2389,13 +2389,13 @@
         <v>124</v>
       </c>
       <c r="B122" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C122" t="n">
         <v>0.0</v>
       </c>
       <c r="D122" t="n">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="123">
@@ -2403,7 +2403,7 @@
         <v>125</v>
       </c>
       <c r="B123" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C123" t="n">
         <v>0.0</v>
@@ -2417,7 +2417,7 @@
         <v>126</v>
       </c>
       <c r="B124" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C124" t="n">
         <v>0.0</v>
@@ -2431,7 +2431,7 @@
         <v>127</v>
       </c>
       <c r="B125" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C125" t="n">
         <v>0.0</v>
@@ -2445,7 +2445,7 @@
         <v>128</v>
       </c>
       <c r="B126" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C126" t="n">
         <v>0.0</v>
@@ -2459,13 +2459,13 @@
         <v>129</v>
       </c>
       <c r="B127" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C127" t="n">
         <v>0.0</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="128">
@@ -2473,7 +2473,7 @@
         <v>130</v>
       </c>
       <c r="B128" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C128" t="n">
         <v>0.0</v>
@@ -2487,7 +2487,7 @@
         <v>131</v>
       </c>
       <c r="B129" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C129" t="n">
         <v>0.0</v>
@@ -2501,7 +2501,7 @@
         <v>132</v>
       </c>
       <c r="B130" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C130" t="n">
         <v>0.0</v>
@@ -2515,7 +2515,7 @@
         <v>133</v>
       </c>
       <c r="B131" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C131" t="n">
         <v>0.0</v>
@@ -2529,7 +2529,7 @@
         <v>134</v>
       </c>
       <c r="B132" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C132" t="n">
         <v>0.0</v>
@@ -2543,7 +2543,7 @@
         <v>135</v>
       </c>
       <c r="B133" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C133" t="n">
         <v>0.0</v>
@@ -2557,7 +2557,7 @@
         <v>136</v>
       </c>
       <c r="B134" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C134" t="n">
         <v>0.0</v>
@@ -2571,13 +2571,13 @@
         <v>137</v>
       </c>
       <c r="B135" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="C135" t="n">
         <v>0.0</v>
       </c>
       <c r="D135" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="136">
@@ -2585,13 +2585,13 @@
         <v>138</v>
       </c>
       <c r="B136" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="C136" t="n">
         <v>0.0</v>
       </c>
       <c r="D136" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="137">
@@ -2599,7 +2599,7 @@
         <v>139</v>
       </c>
       <c r="B137" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C137" t="n">
         <v>0.0</v>
@@ -2613,13 +2613,13 @@
         <v>140</v>
       </c>
       <c r="B138" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C138" t="n">
         <v>1.0</v>
       </c>
-      <c r="C138" t="n">
-        <v>0.0</v>
-      </c>
       <c r="D138" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="139">
@@ -2627,13 +2627,13 @@
         <v>141</v>
       </c>
       <c r="B139" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C139" t="n">
         <v>0.0</v>
       </c>
       <c r="D139" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="140">
@@ -2641,7 +2641,7 @@
         <v>142</v>
       </c>
       <c r="B140" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C140" t="n">
         <v>0.0</v>
@@ -2655,13 +2655,13 @@
         <v>143</v>
       </c>
       <c r="B141" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C141" t="n">
         <v>0.0</v>
       </c>
       <c r="D141" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="142">
@@ -2669,7 +2669,7 @@
         <v>144</v>
       </c>
       <c r="B142" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C142" t="n">
         <v>0.0</v>
@@ -2683,13 +2683,13 @@
         <v>145</v>
       </c>
       <c r="B143" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C143" t="n">
         <v>0.0</v>
       </c>
       <c r="D143" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="144">
@@ -2697,7 +2697,7 @@
         <v>146</v>
       </c>
       <c r="B144" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C144" t="n">
         <v>0.0</v>
@@ -2711,7 +2711,7 @@
         <v>147</v>
       </c>
       <c r="B145" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C145" t="n">
         <v>0.0</v>
@@ -2725,7 +2725,7 @@
         <v>148</v>
       </c>
       <c r="B146" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C146" t="n">
         <v>0.0</v>
@@ -2739,7 +2739,7 @@
         <v>149</v>
       </c>
       <c r="B147" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C147" t="n">
         <v>0.0</v>
@@ -2753,7 +2753,7 @@
         <v>150</v>
       </c>
       <c r="B148" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C148" t="n">
         <v>0.0</v>
@@ -2767,7 +2767,7 @@
         <v>151</v>
       </c>
       <c r="B149" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C149" t="n">
         <v>0.0</v>
@@ -2781,7 +2781,7 @@
         <v>152</v>
       </c>
       <c r="B150" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C150" t="n">
         <v>0.0</v>
@@ -2795,7 +2795,7 @@
         <v>153</v>
       </c>
       <c r="B151" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C151" t="n">
         <v>0.0</v>
@@ -2809,7 +2809,7 @@
         <v>154</v>
       </c>
       <c r="B152" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C152" t="n">
         <v>0.0</v>
@@ -2823,7 +2823,7 @@
         <v>155</v>
       </c>
       <c r="B153" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C153" t="n">
         <v>0.0</v>
@@ -2837,7 +2837,7 @@
         <v>156</v>
       </c>
       <c r="B154" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C154" t="n">
         <v>0.0</v>
@@ -2851,7 +2851,7 @@
         <v>157</v>
       </c>
       <c r="B155" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C155" t="n">
         <v>0.0</v>
@@ -2865,7 +2865,7 @@
         <v>158</v>
       </c>
       <c r="B156" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C156" t="n">
         <v>0.0</v>
@@ -2879,7 +2879,7 @@
         <v>159</v>
       </c>
       <c r="B157" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C157" t="n">
         <v>0.0</v>
@@ -2893,7 +2893,7 @@
         <v>160</v>
       </c>
       <c r="B158" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C158" t="n">
         <v>0.0</v>
@@ -2907,10 +2907,10 @@
         <v>161</v>
       </c>
       <c r="B159" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C159" t="n">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="D159" t="n">
         <v>0.0</v>
@@ -2921,13 +2921,13 @@
         <v>162</v>
       </c>
       <c r="B160" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="C160" t="n">
         <v>0.0</v>
       </c>
       <c r="D160" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="161">
@@ -2935,7 +2935,7 @@
         <v>163</v>
       </c>
       <c r="B161" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C161" t="n">
         <v>0.0</v>
@@ -2949,13 +2949,13 @@
         <v>164</v>
       </c>
       <c r="B162" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C162" t="n">
         <v>0.0</v>
       </c>
       <c r="D162" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="163">
@@ -2963,13 +2963,13 @@
         <v>165</v>
       </c>
       <c r="B163" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C163" t="n">
         <v>0.0</v>
       </c>
       <c r="D163" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="164">
@@ -2977,13 +2977,13 @@
         <v>166</v>
       </c>
       <c r="B164" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C164" t="n">
         <v>0.0</v>
       </c>
       <c r="D164" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="165">
@@ -2991,7 +2991,7 @@
         <v>167</v>
       </c>
       <c r="B165" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C165" t="n">
         <v>0.0</v>
@@ -3005,13 +3005,13 @@
         <v>168</v>
       </c>
       <c r="B166" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="C166" t="n">
         <v>0.0</v>
       </c>
       <c r="D166" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="167">
@@ -3022,7 +3022,7 @@
         <v>0.0</v>
       </c>
       <c r="C167" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="D167" t="n">
         <v>0.0</v>
@@ -3033,13 +3033,13 @@
         <v>170</v>
       </c>
       <c r="B168" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C168" t="n">
         <v>0.0</v>
       </c>
       <c r="D168" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="169">
@@ -3047,13 +3047,13 @@
         <v>171</v>
       </c>
       <c r="B169" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C169" t="n">
         <v>0.0</v>
       </c>
       <c r="D169" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="170">
@@ -3061,13 +3061,13 @@
         <v>172</v>
       </c>
       <c r="B170" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="C170" t="n">
         <v>0.0</v>
       </c>
       <c r="D170" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="171">
@@ -3075,13 +3075,13 @@
         <v>173</v>
       </c>
       <c r="B171" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="C171" t="n">
         <v>0.0</v>
       </c>
       <c r="D171" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="172">
@@ -3089,13 +3089,13 @@
         <v>174</v>
       </c>
       <c r="B172" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C172" t="n">
         <v>0.0</v>
       </c>
       <c r="D172" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="173">
@@ -3103,13 +3103,13 @@
         <v>175</v>
       </c>
       <c r="B173" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="C173" t="n">
         <v>0.0</v>
       </c>
       <c r="D173" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="174">
@@ -3117,13 +3117,13 @@
         <v>176</v>
       </c>
       <c r="B174" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C174" t="n">
         <v>0.0</v>
       </c>
       <c r="D174" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="175">
@@ -3131,13 +3131,13 @@
         <v>177</v>
       </c>
       <c r="B175" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="C175" t="n">
         <v>0.0</v>
       </c>
       <c r="D175" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="176">
@@ -3145,13 +3145,13 @@
         <v>178</v>
       </c>
       <c r="B176" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="C176" t="n">
         <v>0.0</v>
       </c>
       <c r="D176" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="177">
@@ -3159,7 +3159,7 @@
         <v>179</v>
       </c>
       <c r="B177" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C177" t="n">
         <v>0.0</v>
@@ -3173,7 +3173,7 @@
         <v>180</v>
       </c>
       <c r="B178" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C178" t="n">
         <v>0.0</v>
@@ -3187,7 +3187,7 @@
         <v>181</v>
       </c>
       <c r="B179" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C179" t="n">
         <v>0.0</v>
@@ -3201,10 +3201,10 @@
         <v>182</v>
       </c>
       <c r="B180" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C180" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="D180" t="n">
         <v>0.0</v>
@@ -3215,7 +3215,7 @@
         <v>183</v>
       </c>
       <c r="B181" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C181" t="n">
         <v>0.0</v>
@@ -3229,7 +3229,7 @@
         <v>184</v>
       </c>
       <c r="B182" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C182" t="n">
         <v>0.0</v>
@@ -3243,7 +3243,7 @@
         <v>185</v>
       </c>
       <c r="B183" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C183" t="n">
         <v>0.0</v>
@@ -3257,10 +3257,10 @@
         <v>186</v>
       </c>
       <c r="B184" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="C184" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D184" t="n">
         <v>0.0</v>
@@ -3274,7 +3274,7 @@
         <v>0.0</v>
       </c>
       <c r="C185" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="D185" t="n">
         <v>0.0</v>
@@ -3285,7 +3285,7 @@
         <v>188</v>
       </c>
       <c r="B186" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C186" t="n">
         <v>0.0</v>
@@ -3299,7 +3299,7 @@
         <v>189</v>
       </c>
       <c r="B187" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C187" t="n">
         <v>0.0</v>
@@ -3313,13 +3313,13 @@
         <v>190</v>
       </c>
       <c r="B188" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C188" t="n">
         <v>0.0</v>
       </c>
       <c r="D188" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="189">
@@ -3327,7 +3327,7 @@
         <v>191</v>
       </c>
       <c r="B189" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C189" t="n">
         <v>0.0</v>
@@ -3341,7 +3341,7 @@
         <v>192</v>
       </c>
       <c r="B190" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C190" t="n">
         <v>0.0</v>
@@ -3355,7 +3355,7 @@
         <v>193</v>
       </c>
       <c r="B191" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C191" t="n">
         <v>0.0</v>
@@ -3369,10 +3369,10 @@
         <v>194</v>
       </c>
       <c r="B192" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C192" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="D192" t="n">
         <v>0.0</v>
@@ -3383,13 +3383,13 @@
         <v>195</v>
       </c>
       <c r="B193" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="C193" t="n">
         <v>0.0</v>
       </c>
       <c r="D193" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="194">
@@ -3397,7 +3397,7 @@
         <v>196</v>
       </c>
       <c r="B194" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C194" t="n">
         <v>0.0</v>
@@ -3411,7 +3411,7 @@
         <v>197</v>
       </c>
       <c r="B195" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C195" t="n">
         <v>0.0</v>
@@ -3425,7 +3425,7 @@
         <v>198</v>
       </c>
       <c r="B196" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C196" t="n">
         <v>0.0</v>
@@ -3439,13 +3439,13 @@
         <v>199</v>
       </c>
       <c r="B197" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C197" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D197" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="198">
@@ -3453,13 +3453,13 @@
         <v>200</v>
       </c>
       <c r="B198" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C198" t="n">
         <v>0.0</v>
       </c>
       <c r="D198" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="199">
@@ -3467,13 +3467,13 @@
         <v>201</v>
       </c>
       <c r="B199" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="C199" t="n">
         <v>0.0</v>
       </c>
       <c r="D199" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="200">
@@ -3481,7 +3481,7 @@
         <v>202</v>
       </c>
       <c r="B200" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C200" t="n">
         <v>0.0</v>
@@ -3498,7 +3498,7 @@
         <v>0.0</v>
       </c>
       <c r="C201" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="D201" t="n">
         <v>0.0</v>
@@ -3509,13 +3509,13 @@
         <v>204</v>
       </c>
       <c r="B202" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="C202" t="n">
         <v>0.0</v>
       </c>
       <c r="D202" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>